<commit_message>
Updated Use Case Diagram
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A041CE02-0F5C-4C80-8298-2BEE70B4BF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375DF775-0BC4-4830-96F6-C3601487EB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
-    <sheet name="01. Generate Voucher" sheetId="2" r:id="rId2"/>
-    <sheet name="02. Issue Warning Letter" sheetId="17" r:id="rId3"/>
-    <sheet name="03. Create Customer Membership " sheetId="18" r:id="rId4"/>
-    <sheet name="04. Create New Employee" sheetId="19" r:id="rId5"/>
-    <sheet name="05. Purchase New Facilities and" sheetId="20" r:id="rId6"/>
-    <sheet name="06. Change Working Time" sheetId="21" r:id="rId7"/>
-    <sheet name="07. Adjust Employee Salary" sheetId="22" r:id="rId8"/>
-    <sheet name="08. Manage Movie Schedule" sheetId="24" r:id="rId9"/>
+    <sheet name="01. Accept or Reject Resignatio" sheetId="2" r:id="rId2"/>
+    <sheet name="02. Create Broken Facility Repo" sheetId="17" r:id="rId3"/>
+    <sheet name="03. Propose Warning Letter" sheetId="18" r:id="rId4"/>
+    <sheet name="04. Set Employee Working Time" sheetId="19" r:id="rId5"/>
+    <sheet name="05. Create Membership" sheetId="20" r:id="rId6"/>
+    <sheet name="06. Create Ticket" sheetId="21" r:id="rId7"/>
+    <sheet name="07. Create Food Beverage Order" sheetId="22" r:id="rId8"/>
+    <sheet name="08. Create Movie Schedule" sheetId="24" r:id="rId9"/>
     <sheet name="09. Request Personal Leave" sheetId="25" r:id="rId10"/>
     <sheet name="10. Serve Customer Movie Ticket" sheetId="26" r:id="rId11"/>
   </sheets>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="53">
   <si>
     <t>CONTENT</t>
   </si>
@@ -151,67 +151,77 @@
     <t>BACK TO TABLE OF CONTENT</t>
   </si>
   <si>
-    <t>Purchase New Facilities and Equipments</t>
-  </si>
-  <si>
-    <t>Storage Department</t>
-  </si>
-  <si>
-    <t>Storage department is also in charge of purchasing new facilities and equipment requested by other departments and has been approved by the accounting and finance departments.</t>
-  </si>
-  <si>
-    <t>Purchase facility and equipment</t>
-  </si>
-  <si>
-    <t>Accounting and Finance Department</t>
-  </si>
-  <si>
-    <t>Change Working Time</t>
-  </si>
-  <si>
-    <t>A facility or equipment is being requested by other department</t>
-  </si>
-  <si>
-    <t>1. Storage department views the facilities and equipments lists.</t>
-  </si>
-  <si>
-    <t>1.1. System displays the list of the facilities and equipments, including the details, such as who, when, and where the facility and equipment were last used and the quantity of it.</t>
-  </si>
-  <si>
-    <t>3. Accounting and Finance Department views and verifies the request purchase item list.</t>
-  </si>
-  <si>
-    <t>4.1. System stores the new facilities and equipments in database.</t>
-  </si>
-  <si>
-    <t>2.1. Basic request purchase item data are incomplete.
-2.2. If the accounting and finance department rejects the request purchase item, notify the respective department that the request is being rejected.</t>
-  </si>
-  <si>
-    <t>2. Storage department submit requested purchase item information to Accounting and Finance Department with details as following (facility/equipment name, quantity, purpose, etc.).</t>
-  </si>
-  <si>
-    <t>Storage department desires to purchase a new facility or equipment.</t>
-  </si>
-  <si>
-    <t>When the other departments requested puchasing new facilities and equipment and has been approved by the accounting and finance department.</t>
-  </si>
-  <si>
-    <t>- Storage department will buy the requested item.
-- Storage department record purchase data.
-- Facility and equipment will be labelled, saved, and records to system.
-- Notify the department that the requested item is already bought.</t>
-  </si>
-  <si>
-    <t>4. Storage department inserts the new facilities and equipments.</t>
-  </si>
-  <si>
-    <t>3.1. System displays the list of requested purchase item.
-3.2. System notifies storage department about the accounting and finance department's approval, either approved or rejected.</t>
-  </si>
-  <si>
-    <t>2.1. System creates a new purchase request.
-2.2. System sends requested item and fund request to Accounting and Finance Department and asks the Accounting and Finance Department's approval.</t>
+    <t>Propose Warning Letter</t>
+  </si>
+  <si>
+    <t>Set Employee Working Time</t>
+  </si>
+  <si>
+    <t>Create Membership</t>
+  </si>
+  <si>
+    <t>Create Ticket</t>
+  </si>
+  <si>
+    <t>Create Food/Beverage Order</t>
+  </si>
+  <si>
+    <t>Create Movie Schedule</t>
+  </si>
+  <si>
+    <t>Accept/Reject Resignation Request</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Manager accepts or rejects resignation request</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Employee submits resignation letter</t>
+  </si>
+  <si>
+    <t>Employee must know the outcome of the resignation request</t>
+  </si>
+  <si>
+    <t>Manager reviews the resignation request and decides to accept or reject the resignation request</t>
+  </si>
+  <si>
+    <t>Submit Resignation Letter</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Approve/Disapprove Warning Letter</t>
+  </si>
+  <si>
+    <t>Approve/disapprove warning letter</t>
+  </si>
+  <si>
+    <t>Manager approves or disapproves a warning letter</t>
+  </si>
+  <si>
+    <t>Manager sees a warning letter approval request</t>
+  </si>
+  <si>
+    <t>Human Resource Department, Employee</t>
+  </si>
+  <si>
+    <t>Employee violates a rule, Human Resource Department proposes a warning letter</t>
+  </si>
+  <si>
+    <t>Human Resource Department must know the manager's decision, and response accordingly.
+If the warning letter proposal is accepted, the human resource depatment will email the warning letter to the employee and the system will save the warning letter to the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Manager chooses </t>
+  </si>
+  <si>
+    <t>Employee wants to resign, they submitted a resignation request</t>
   </si>
 </sst>
 </file>
@@ -307,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -576,12 +586,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -651,39 +723,39 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -707,6 +779,39 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D94B0A-294A-46CD-80A0-E82950B2698E}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1139,64 +1244,64 @@
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1291,15 +1396,15 @@
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1307,67 +1412,67 @@
         <v>13</v>
       </c>
       <c r="B3" s="38"/>
-      <c r="C3" s="28"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1378,22 +1483,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
@@ -1447,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA9D18-1CA4-4871-85B2-18BB43F4E55C}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,83 +1568,103 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1550,64 +1675,51 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
-    <row r="14" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="14" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B14" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -1615,7 +1727,7 @@
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A22" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
+    <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1624,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FE8960-F0AE-4855-9BA4-1CED20B6740B}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,156 +1752,188 @@
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="52"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
       <c r="B16" s="12"/>
       <c r="C16" s="18"/>
     </row>
-    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
       <c r="B17" s="12"/>
       <c r="C17" s="18"/>
     </row>
-    <row r="18" spans="1:4" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
       <c r="B18" s="12"/>
       <c r="C18" s="18"/>
     </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="15"/>
+    </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="B19:C19"/>
+  <mergeCells count="13">
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1799,10 +1943,11 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:C12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A24" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{98A3338B-B1EA-4D93-B3FF-F333EECF1661}"/>
+    <hyperlink ref="A26" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{98A3338B-B1EA-4D93-B3FF-F333EECF1661}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1813,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,83 +1972,85 @@
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1914,17 +2061,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -1980,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6806F9-C482-4A96-BD07-0DB8CFD37B42}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,83 +2141,85 @@
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2081,17 +2230,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -2148,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED55F7-F44D-46F6-ADD5-ADA5945F102D}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,155 +2311,115 @@
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="33"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>37</v>
-      </c>
+      <c r="A12" s="32"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>47</v>
-      </c>
+      <c r="A13" s="32"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>46</v>
-      </c>
+      <c r="A14" s="32"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>39</v>
-      </c>
+      <c r="A15" s="32"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>40</v>
-      </c>
+      <c r="B16" s="25"/>
       <c r="C16" s="26"/>
       <c r="D16" s="15"/>
     </row>
@@ -2358,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D1CD4-D048-44CE-AE14-06222F52D34C}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2372,85 +2481,85 @@
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2461,22 +2570,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
@@ -2532,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B5A171-C8CF-457E-9DF8-6E96F6236BCA}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,83 +2655,85 @@
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2633,17 +2744,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="16"/>
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -2699,8 +2810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC3CBF5-E167-48E6-8768-D133250BF158}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,15 +2824,17 @@
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2729,67 +2842,67 @@
         <v>13</v>
       </c>
       <c r="B3" s="38"/>
-      <c r="C3" s="28"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2800,22 +2913,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12"/>
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>

</xml_diff>

<commit_message>
Declared Use Case Description
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375DF775-0BC4-4830-96F6-C3601487EB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D65D70-B8B8-416A-8BB7-1235361A05D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
-    <sheet name="01. Accept or Reject Resignatio" sheetId="2" r:id="rId2"/>
-    <sheet name="02. Create Broken Facility Repo" sheetId="17" r:id="rId3"/>
-    <sheet name="03. Propose Warning Letter" sheetId="18" r:id="rId4"/>
-    <sheet name="04. Set Employee Working Time" sheetId="19" r:id="rId5"/>
-    <sheet name="05. Create Membership" sheetId="20" r:id="rId6"/>
+    <sheet name="01. Propose Warning Letter" sheetId="18" r:id="rId2"/>
+    <sheet name="02. Accept or Reject Resignatio" sheetId="2" r:id="rId3"/>
+    <sheet name="03. Approve or Disapprove Warni" sheetId="17" r:id="rId4"/>
+    <sheet name="04. Add Employee" sheetId="19" r:id="rId5"/>
+    <sheet name="05. Update Employee Salary" sheetId="20" r:id="rId6"/>
     <sheet name="06. Create Ticket" sheetId="21" r:id="rId7"/>
     <sheet name="07. Create Food Beverage Order" sheetId="22" r:id="rId8"/>
-    <sheet name="08. Create Movie Schedule" sheetId="24" r:id="rId9"/>
-    <sheet name="09. Request Personal Leave" sheetId="25" r:id="rId10"/>
-    <sheet name="10. Serve Customer Movie Ticket" sheetId="26" r:id="rId11"/>
+    <sheet name="08. Create Membership" sheetId="24" r:id="rId9"/>
+    <sheet name="09. Add Supplier" sheetId="25" r:id="rId10"/>
+    <sheet name="10. Add Advertisement Partner" sheetId="26" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="63">
   <si>
     <t>CONTENT</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Propose Warning Letter</t>
   </si>
   <si>
-    <t>Set Employee Working Time</t>
-  </si>
-  <si>
     <t>Create Membership</t>
   </si>
   <si>
@@ -166,30 +163,18 @@
     <t>Create Food/Beverage Order</t>
   </si>
   <si>
-    <t>Create Movie Schedule</t>
-  </si>
-  <si>
     <t>Accept/Reject Resignation Request</t>
   </si>
   <si>
-    <t>Employee</t>
-  </si>
-  <si>
     <t>Manager accepts or rejects resignation request</t>
   </si>
   <si>
     <t>Manager</t>
   </si>
   <si>
-    <t>Employee submits resignation letter</t>
-  </si>
-  <si>
     <t>Employee must know the outcome of the resignation request</t>
   </si>
   <si>
-    <t>Manager reviews the resignation request and decides to accept or reject the resignation request</t>
-  </si>
-  <si>
     <t>Submit Resignation Letter</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
   </si>
   <si>
     <t>Manager approves or disapproves a warning letter</t>
-  </si>
-  <si>
-    <t>Manager sees a warning letter approval request</t>
   </si>
   <si>
     <t>Human Resource Department, Employee</t>
@@ -218,10 +200,58 @@
 If the warning letter proposal is accepted, the human resource depatment will email the warning letter to the employee and the system will save the warning letter to the database</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Manager chooses </t>
-  </si>
-  <si>
-    <t>Employee wants to resign, they submitted a resignation request</t>
+    <t>Employee violates a rule, human resource department proposes a warning letter, manager sees the warning letter approval request.</t>
+  </si>
+  <si>
+    <t>1. Manager updates the warning letter proposal status</t>
+  </si>
+  <si>
+    <t>1.1 System responds accordingly, if the proposal is accepted</t>
+  </si>
+  <si>
+    <t>Human resource department proposes a warning letter</t>
+  </si>
+  <si>
+    <t>Employee did a violation</t>
+  </si>
+  <si>
+    <t>Human resource department</t>
+  </si>
+  <si>
+    <t>Warning letter proposal must be created and saved</t>
+  </si>
+  <si>
+    <t>1. Human resource department fills in the necessary information of a warning letter proposal</t>
+  </si>
+  <si>
+    <t>1.1 System creates a new warning letter proposal</t>
+  </si>
+  <si>
+    <t>Necessary warning letter proposal information are incomplete</t>
+  </si>
+  <si>
+    <t>Human resource department creates a warning letter proposal by filling necessary information</t>
+  </si>
+  <si>
+    <t>Resignation request must exist</t>
+  </si>
+  <si>
+    <t>Employee submitted a resignation request</t>
+  </si>
+  <si>
+    <t>Employee, Human Resource Department, Accounting and Finance</t>
+  </si>
+  <si>
+    <t>Add Employee</t>
+  </si>
+  <si>
+    <t>Update Employee Salary</t>
+  </si>
+  <si>
+    <t>Add Supplier</t>
+  </si>
+  <si>
+    <t>Add Advertisement Partner</t>
   </si>
 </sst>
 </file>
@@ -317,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -648,12 +678,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -717,43 +799,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -780,38 +895,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1216,7 +1310,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,22 +1323,24 @@
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="37"/>
       <c r="D3" s="15"/>
     </row>
@@ -1252,7 +1348,7 @@
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
@@ -1260,7 +1356,7 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="37"/>
       <c r="D5" s="15"/>
     </row>
@@ -1268,44 +1364,44 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="29"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="37"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="50" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1316,17 +1412,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -1334,8 +1430,8 @@
       <c r="A15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1382,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79415FA7-6CDB-42D8-A113-D2105F582302}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,30 +1492,32 @@
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
@@ -1427,52 +1525,52 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1483,22 +1581,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
@@ -1506,8 +1604,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1551,11 +1649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA9D18-1CA4-4871-85B2-18BB43F4E55C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,103 +1666,103 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="28"/>
+      <c r="B3" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>52</v>
+      <c r="B4" s="36" t="s">
+        <v>49</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="30"/>
+      <c r="B10" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1674,24 +1772,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="60"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="47"/>
+      <c r="B14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="39"/>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1712,22 +1814,24 @@
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
+    <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{3EF5B233-17BD-4CD6-9AA2-399E784F1A74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1735,11 +1839,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FE8960-F0AE-4855-9BA4-1CED20B6740B}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA9D18-1CA4-4871-85B2-18BB43F4E55C}">
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,202 +1856,164 @@
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="28"/>
+      <c r="B3" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>47</v>
+      <c r="B4" s="36" t="s">
+        <v>57</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="52"/>
+      <c r="B10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="18"/>
-    </row>
-    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="18"/>
-    </row>
-    <row r="20" spans="1:4" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="18"/>
-    </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="B14" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B1:C1"/>
+  <mergeCells count="12">
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:C12"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A26" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{98A3338B-B1EA-4D93-B3FF-F333EECF1661}"/>
+    <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1955,7 +2021,236 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FE8960-F0AE-4855-9BA4-1CED20B6740B}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="18"/>
+    </row>
+    <row r="18" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="18"/>
+    </row>
+    <row r="22" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:C13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A27" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{98A3338B-B1EA-4D93-B3FF-F333EECF1661}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6806F9-C482-4A96-BD07-0DB8CFD37B42}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1970,256 +2265,87 @@
   <sheetData>
     <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A20" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{3EF5B233-17BD-4CD6-9AA2-399E784F1A74}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6806F9-C482-4A96-BD07-0DB8CFD37B42}">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="3" width="50.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2230,17 +2356,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -2248,8 +2374,8 @@
       <c r="A15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2298,7 +2424,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,32 +2437,32 @@
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
@@ -2344,74 +2470,74 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
@@ -2419,8 +2545,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2481,32 +2607,32 @@
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
@@ -2514,52 +2640,52 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2570,22 +2696,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
@@ -2593,8 +2719,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2655,32 +2781,32 @@
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
@@ -2688,52 +2814,52 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2744,17 +2870,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="16"/>
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -2762,8 +2888,8 @@
       <c r="A15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2811,7 +2937,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,32 +2950,32 @@
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="34"/>
+      <c r="B1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="15"/>
     </row>
@@ -2857,52 +2983,52 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2913,22 +3039,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12"/>
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="12"/>
       <c r="C15" s="18"/>
     </row>
@@ -2936,8 +3062,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Started use case description
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D65D70-B8B8-416A-8BB7-1235361A05D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B2D0B9-971C-47B2-912A-39809ABCE9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
   <si>
     <t>CONTENT</t>
   </si>
@@ -169,79 +169,12 @@
     <t>Manager accepts or rejects resignation request</t>
   </si>
   <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Employee must know the outcome of the resignation request</t>
-  </si>
-  <si>
-    <t>Submit Resignation Letter</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Approve/Disapprove Warning Letter</t>
   </si>
   <si>
-    <t>Approve/disapprove warning letter</t>
-  </si>
-  <si>
-    <t>Manager approves or disapproves a warning letter</t>
-  </si>
-  <si>
-    <t>Human Resource Department, Employee</t>
-  </si>
-  <si>
-    <t>Employee violates a rule, Human Resource Department proposes a warning letter</t>
-  </si>
-  <si>
-    <t>Human Resource Department must know the manager's decision, and response accordingly.
-If the warning letter proposal is accepted, the human resource depatment will email the warning letter to the employee and the system will save the warning letter to the database</t>
-  </si>
-  <si>
-    <t>Employee violates a rule, human resource department proposes a warning letter, manager sees the warning letter approval request.</t>
-  </si>
-  <si>
-    <t>1. Manager updates the warning letter proposal status</t>
-  </si>
-  <si>
-    <t>1.1 System responds accordingly, if the proposal is accepted</t>
-  </si>
-  <si>
     <t>Human resource department proposes a warning letter</t>
   </si>
   <si>
-    <t>Employee did a violation</t>
-  </si>
-  <si>
-    <t>Human resource department</t>
-  </si>
-  <si>
-    <t>Warning letter proposal must be created and saved</t>
-  </si>
-  <si>
-    <t>1. Human resource department fills in the necessary information of a warning letter proposal</t>
-  </si>
-  <si>
-    <t>1.1 System creates a new warning letter proposal</t>
-  </si>
-  <si>
-    <t>Necessary warning letter proposal information are incomplete</t>
-  </si>
-  <si>
-    <t>Human resource department creates a warning letter proposal by filling necessary information</t>
-  </si>
-  <si>
-    <t>Resignation request must exist</t>
-  </si>
-  <si>
-    <t>Employee submitted a resignation request</t>
-  </si>
-  <si>
-    <t>Employee, Human Resource Department, Accounting and Finance</t>
-  </si>
-  <si>
     <t>Add Employee</t>
   </si>
   <si>
@@ -252,6 +185,60 @@
   </si>
   <si>
     <t>Add Advertisement Partner</t>
+  </si>
+  <si>
+    <t>Approve or Disapprove Warning Letter</t>
+  </si>
+  <si>
+    <t>Manager approves or disapproves warning letter proposal</t>
+  </si>
+  <si>
+    <t>Human resource department adds a new employee to the system</t>
+  </si>
+  <si>
+    <t>Finance and accounting department changes employee salary</t>
+  </si>
+  <si>
+    <t>Movie front office division serves customer who wants to buy a ticket</t>
+  </si>
+  <si>
+    <t>Café front office department serves customer who want to order snacks</t>
+  </si>
+  <si>
+    <t>Movie front office division serves customer who wants to become a member</t>
+  </si>
+  <si>
+    <t>External department adds a new advertisement partner</t>
+  </si>
+  <si>
+    <t>External division adds a new supplier</t>
+  </si>
+  <si>
+    <t>Employee violated company rule</t>
+  </si>
+  <si>
+    <t>Manager sees/is notified by a resignation request</t>
+  </si>
+  <si>
+    <t>Manager sees/is notified by a warning letter approval request</t>
+  </si>
+  <si>
+    <t>The human resource department accepted new employee/employees</t>
+  </si>
+  <si>
+    <t>Manager accepts salary change request by human resource department</t>
+  </si>
+  <si>
+    <t>Customer wants to buy a ticket, a movie front office employee serves them</t>
+  </si>
+  <si>
+    <t>Customer wants to buy food/beverages, a café front office employee serves them</t>
+  </si>
+  <si>
+    <t>Customer wants to be a member, an employee serves them</t>
+  </si>
+  <si>
+    <t>External department wants to add a new supplier</t>
   </si>
 </sst>
 </file>
@@ -802,17 +789,53 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -820,30 +843,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -894,18 +893,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1309,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D94B0A-294A-46CD-80A0-E82950B2698E}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,85 +1310,91 @@
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="54"/>
+      <c r="B1" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="56"/>
+      <c r="B2" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="60"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="B3" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="54" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1412,17 +1405,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="12"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="12"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="12"/>
       <c r="C14" s="18"/>
     </row>
@@ -1430,8 +1423,8 @@
       <c r="A15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1478,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79415FA7-6CDB-42D8-A113-D2105F582302}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,81 +1485,85 @@
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1604,8 +1601,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1653,7 +1650,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,99 +1663,87 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="35"/>
+      <c r="B3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="29"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1774,26 +1759,20 @@
     </row>
     <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>53</v>
-      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="60"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="41"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="39"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1822,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,97 +1835,87 @@
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="29"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,10 +1943,8 @@
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="31"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1999,18 +1966,18 @@
     <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
@@ -2025,7 +1992,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,115 +2005,105 @@
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="35"/>
+      <c r="B3" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="44"/>
+      <c r="B4" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="48"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="29"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="44"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2162,12 +2119,8 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
-      <c r="B15" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>47</v>
-      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
@@ -2203,8 +2156,8 @@
       <c r="A22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2207,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,81 +2220,87 @@
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2374,8 +2333,8 @@
       <c r="A15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2423,7 +2382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED55F7-F44D-46F6-ADD5-ADA5945F102D}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
@@ -2437,81 +2396,87 @@
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,8 +2510,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2593,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D1CD4-D048-44CE-AE14-06222F52D34C}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="117" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,81 +2572,87 @@
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2719,8 +2690,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2767,8 +2738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B5A171-C8CF-457E-9DF8-6E96F6236BCA}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,81 +2752,87 @@
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2888,8 +2865,8 @@
       <c r="A15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2937,7 +2914,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,81 +2927,87 @@
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3062,8 +3045,8 @@
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Major Progress on Use Case Description
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B2D0B9-971C-47B2-912A-39809ABCE9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DA626F-BF60-43D6-B36C-4E36EA5E5D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="100">
   <si>
     <t>CONTENT</t>
   </si>
@@ -226,9 +226,6 @@
     <t>The human resource department accepted new employee/employees</t>
   </si>
   <si>
-    <t>Manager accepts salary change request by human resource department</t>
-  </si>
-  <si>
     <t>Customer wants to buy a ticket, a movie front office employee serves them</t>
   </si>
   <si>
@@ -239,6 +236,144 @@
   </si>
   <si>
     <t>External department wants to add a new supplier</t>
+  </si>
+  <si>
+    <t>Manager accepts salary change request by human resource department, the system forwards the data for further processing</t>
+  </si>
+  <si>
+    <t>External department wants to add a new advertisement partner</t>
+  </si>
+  <si>
+    <t>Human resource department</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Accounting and finance department</t>
+  </si>
+  <si>
+    <t>Movie department front office division</t>
+  </si>
+  <si>
+    <t>Café department front office division</t>
+  </si>
+  <si>
+    <t>External department</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Submit Resignation Letter</t>
+  </si>
+  <si>
+    <t>Accept/Reject Salary Change, Propose Salary Change</t>
+  </si>
+  <si>
+    <t>View Shedule, Create Schedule, Update Schedule</t>
+  </si>
+  <si>
+    <t>View Food and Beverages</t>
+  </si>
+  <si>
+    <t>Manager, Employee</t>
+  </si>
+  <si>
+    <t>Employee, Human Resource, Accounting and finance</t>
+  </si>
+  <si>
+    <t>Human resource, Employee</t>
+  </si>
+  <si>
+    <t>Manager, Accounting and Finance</t>
+  </si>
+  <si>
+    <t>Manager, Employee, Human resource</t>
+  </si>
+  <si>
+    <t>Accounting and finance</t>
+  </si>
+  <si>
+    <t>Accounting and finance, External</t>
+  </si>
+  <si>
+    <t>Promotion and event, Manager</t>
+  </si>
+  <si>
+    <t>Café kitchen division, Accounting and finance</t>
+  </si>
+  <si>
+    <t>Warning letter subsystem must be available</t>
+  </si>
+  <si>
+    <t>Resignation request must exist.
+Resignation request subsystem must exist.</t>
+  </si>
+  <si>
+    <t>Warning letter must exist
+Warning letter subsytem must exist</t>
+  </si>
+  <si>
+    <t>Employee subsystem must exist</t>
+  </si>
+  <si>
+    <t>Employee must exist
+Employee subsystem must exist</t>
+  </si>
+  <si>
+    <t>Membership subsystem must exist</t>
+  </si>
+  <si>
+    <t>Supplier subsystem must exist</t>
+  </si>
+  <si>
+    <t>Advertisement partner subsystem must exist</t>
+  </si>
+  <si>
+    <t>Warning letter must be created and saved</t>
+  </si>
+  <si>
+    <t>Resignation request status must be updated and saved</t>
+  </si>
+  <si>
+    <t>Warning letter status must be updated and saved</t>
+  </si>
+  <si>
+    <t>Employee must be created and saved</t>
+  </si>
+  <si>
+    <t>Employee salary must be updates and saved</t>
+  </si>
+  <si>
+    <t>Ticket must be created, saved, and printed
+Available movie tickets must be updated
+Payment must be authenticated</t>
+  </si>
+  <si>
+    <t>Ticket subsystem must exist
+Movie schedule must be available
+Payment authorization services must be available</t>
+  </si>
+  <si>
+    <t>Food and beverages order subsystem must exist
+Food and beverge stock must be available
+Payment authorization services must be available</t>
+  </si>
+  <si>
+    <t>Order must be created and saved
+Receipt must be printed
+Available stock must be updated
+Payment must be authenticated</t>
+  </si>
+  <si>
+    <t>Membership must be created and saved</t>
+  </si>
+  <si>
+    <t>Supplier must be created and saved</t>
+  </si>
+  <si>
+    <t>Advertisement partner must be created and saved</t>
   </si>
 </sst>
 </file>
@@ -1296,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D94B0A-294A-46CD-80A0-E82950B2698E}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1475,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="15"/>
@@ -1357,7 +1492,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>65</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -1365,7 +1502,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -1373,7 +1512,9 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>79</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
@@ -1381,7 +1522,9 @@
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="37" t="s">
+        <v>86</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
@@ -1389,7 +1532,9 @@
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>98</v>
+      </c>
       <c r="C10" s="35"/>
       <c r="D10" s="15"/>
     </row>
@@ -1472,7 +1617,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,11 +1659,13 @@
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="34" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
@@ -1530,7 +1677,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>65</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -1538,7 +1687,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -1546,7 +1697,9 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>76</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
@@ -1554,7 +1707,9 @@
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="37" t="s">
+        <v>87</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
@@ -1562,7 +1717,9 @@
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>99</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -1649,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" activeCellId="1" sqref="C11 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1867,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -1718,7 +1877,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -1726,7 +1887,9 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>71</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
@@ -1734,7 +1897,9 @@
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="37" t="s">
+        <v>80</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
@@ -1742,7 +1907,9 @@
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="37" t="s">
+        <v>88</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -1822,7 +1989,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +2049,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>61</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -1890,7 +2059,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>67</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -1898,15 +2069,19 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>72</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
@@ -1914,7 +2089,9 @@
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="37" t="s">
+        <v>89</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -1966,18 +2143,18 @@
     <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
@@ -1992,7 +2169,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C5"/>
+      <selection activeCell="A14" sqref="A14:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,7 +2235,9 @@
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -2066,7 +2245,9 @@
       <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
@@ -2074,15 +2255,19 @@
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="37" t="s">
+        <v>73</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="34" t="s">
+        <v>82</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -2090,17 +2275,19 @@
       <c r="A11" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="47" t="s">
+        <v>90</v>
+      </c>
       <c r="C11" s="48"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="45"/>
       <c r="B12" s="49"/>
       <c r="C12" s="50"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
       <c r="B13" s="51"/>
       <c r="C13" s="52"/>
@@ -2207,7 +2394,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2454,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -2275,7 +2464,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -2283,7 +2474,9 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>74</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
@@ -2291,15 +2484,19 @@
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="37" t="s">
+        <v>83</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>91</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -2382,8 +2579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED55F7-F44D-46F6-ADD5-ADA5945F102D}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,7 +2623,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="15"/>
@@ -2443,7 +2640,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>62</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -2451,7 +2650,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>68</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -2459,23 +2660,29 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>75</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34" t="s">
+        <v>84</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>92</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -2483,8 +2690,12 @@
       <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
@@ -2558,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D1CD4-D048-44CE-AE14-06222F52D34C}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2602,7 +2813,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="15"/>
@@ -2619,7 +2830,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>63</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -2627,7 +2840,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>69</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -2635,23 +2850,29 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>76</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34" t="s">
+        <v>94</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="34" t="s">
+        <v>93</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -2738,8 +2959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B5A171-C8CF-457E-9DF8-6E96F6236BCA}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView topLeftCell="A7" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,7 +3003,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="15"/>
@@ -2799,7 +3020,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>64</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -2807,7 +3030,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>70</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -2815,23 +3040,29 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>77</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34" t="s">
+        <v>95</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>96</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
@@ -2914,7 +3145,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,7 +3188,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="15"/>
@@ -2974,7 +3205,9 @@
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>63</v>
+      </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
@@ -2982,7 +3215,9 @@
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
@@ -2990,23 +3225,29 @@
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>78</v>
+      </c>
       <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>97</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>

</xml_diff>

<commit_message>
Added Use Case Description
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A1112-2E7E-4399-A476-DCD720A5C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148A9725-FA3A-4DE2-9AF6-82C056EE944F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="141">
   <si>
     <t>CONTENT</t>
   </si>
@@ -349,21 +349,11 @@
     <t>Advertisement partner must be created and saved</t>
   </si>
   <si>
-    <t>1.1 System gets all employees
-2.1 System displays a form
-3.1 System will create and save a new warning letter proposal</t>
-  </si>
-  <si>
     <t>1. Manager prompts to view resignation requests
 2. Manager selects a resignation request
 3. Manager updates the status of the resignation request</t>
   </si>
   <si>
-    <t>1.1 System gets and displays the resignation requests
-2.1 System gets the resignation letter and saves it in the manager's device
-3. 1 System updates and saves the status change</t>
-  </si>
-  <si>
     <t>1. Human resource department prompts to view employees
 2. Human resource departmen selects an employee to report
 3. Human resource department inputs the reason for the warning letter(reason)</t>
@@ -374,15 +364,6 @@
 3. Manager updates the warning letter status </t>
   </si>
   <si>
-    <t>1.1 System gets warning letters
-2.1 System displays the detaild of the warning letter proposal, such as reason
-3.1 System updates and saves the warning letter status</t>
-  </si>
-  <si>
-    <t>1. Human resource prompts to add a new employee
-2. Human resource fills in necesarry employee information(name, gender, department, email, phone, salary, address, date of birth)</t>
-  </si>
-  <si>
     <t>1.1 System displays a form asking for necessary employee information 
 2.1 System creates and saves a new employee</t>
   </si>
@@ -395,11 +376,143 @@
 2.1 System updates and saves the salary change</t>
   </si>
   <si>
-    <t>1.1 System gets and displays the available movie schedule, along with the available seats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Movie front office prompts to create a ticket
-2. Movie front office selects the movie schedule </t>
+    <t>1. Movie front office prompts to view ongoing movies
+2. Movie front office selects movie
+3. Movie front office selects a schedule
+4. Movie front office selects the seats according to the customer's request
+5. Movie front office selects the payment method and prompts to print ticket</t>
+  </si>
+  <si>
+    <t>1.1 System gets and displays ongoing movies
+2.1 System gets and displays the available schedules for the selected movie
+3.1 System displays the available seats for the selected movie schedule
+4.1 System calculates the total ticket price
+4.2 System displays the total ticket price
+4.3 System displays the available payment methods
+5.1 System prints ticket
+5.2 System saves and records the ticket purchase</t>
+  </si>
+  <si>
+    <t>1. Café front office employee prompts to view available fnb 
+item
+2. Café front office employee selects the available items, according to customer's request
+3. Café front office selects a payment method and prompts to to create order</t>
+  </si>
+  <si>
+    <t>1.1 System gets and displays the available fnb items
+2.1 System calculates the total price
+2.2 System displays the total price
+2.3 System displays the available payment methods
+3.1 System saves and creates the order</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form for creating a new 
+membership
+2.1 System creates and saves new employee</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form to add a new supplier
+2.1 System creates and saves the new supplier</t>
+  </si>
+  <si>
+    <t>1. Movie front office employee prompts to create a new membership
+2. Movie front office enters necessary customer information (name, gender, email, phone number, address, date of birth)</t>
+  </si>
+  <si>
+    <t>1. External department employee prompts to add a new supplier
+2. External department employee fills the necessary information needed to add a new supplier (name, email, phone number, address)</t>
+  </si>
+  <si>
+    <t>1. External department employee prompts to add a new advertisement partner
+2. External department employee fills the necessary informarion to add a new advertisement partner (name, email, phonenumber, address)</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form to create a new advertisement partner
+2.1 System saves and creates the new advertisement partner</t>
+  </si>
+  <si>
+    <t>1.1 System gets all employees data
+2.1 System displays a form
+3.1 System will create and save a new warning letter proposal</t>
+  </si>
+  <si>
+    <t>Human resource department proposes a warning letter by first retrieving a list of employees, then proceeds to select the employee to report along with the reason.</t>
+  </si>
+  <si>
+    <t>Manager retrieves a list of resignation requests, selects one of them and decides to accept or reject the request</t>
+  </si>
+  <si>
+    <t>Manager receives a list of warning letter approval request, selects one of them, and decides to approve or disapprove the warning letter</t>
+  </si>
+  <si>
+    <t>Human resource department adds a new employee by entering basic employee information</t>
+  </si>
+  <si>
+    <t>Accounting and finance department gets a list of employees who salary change is accepted, and proceeds to update the salary based on the list</t>
+  </si>
+  <si>
+    <t>Movie front office division creates ticket by retrieving ongoing movies, selecting a movie, a schedule, seat number, and payment method.</t>
+  </si>
+  <si>
+    <t>Café front office employee creates a fnb order by selecting fnb items and payment type</t>
+  </si>
+  <si>
+    <t>Movie front office creates a new member by filling basic  information</t>
+  </si>
+  <si>
+    <t>External department employee creates and adds a new advertisement partner by filling basic advertisement partner information</t>
+  </si>
+  <si>
+    <t>External department employee creates and adds a new supplier by filling basic supplier  information</t>
+  </si>
+  <si>
+    <t>3.1. Reason is not filled by the human resource department</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1. Human resource prompts to add a new employee
+2. Human resource fills in necesarry employee information(name, gender, department, email, phonenumber, salary, address, date of birth)</t>
+  </si>
+  <si>
+    <t>1.1 System gets and displays the resignation requests
+2.1 System displays the resignation letter
+3. 1 System updates and saves the status change</t>
+  </si>
+  <si>
+    <t>2.1 Employee information(name, gender, department, email, phonenumber, salary, address, date of birth) may be incomplete</t>
+  </si>
+  <si>
+    <t>1.1 The list of employees whose salary change was accepted doesn't exist</t>
+  </si>
+  <si>
+    <t>1.1 System gets warning letter proposals
+2.1 System displays the details of the warning letter proposal, such as reason
+3.1 System updates and saves the warning letter status</t>
+  </si>
+  <si>
+    <t>1.1 the resignation requests doesn’t exist</t>
+  </si>
+  <si>
+    <t>1.1 Warning letter proposals doesn't exist</t>
+  </si>
+  <si>
+    <t>1.1 Ongoing movies doesn't exist
+2.1 Schedule for a particular movie doesn’t exist
+3.1 Available seats for a movie schedule doesn't exist</t>
+  </si>
+  <si>
+    <t>1.1 FnB items doesn't exist</t>
+  </si>
+  <si>
+    <t>2.1 Customer information (name, gender, email, phone number, address, date of birth) may be incomplete</t>
+  </si>
+  <si>
+    <t>2.1 Supplier information (name, email, phone number, address) may be incomplete</t>
+  </si>
+  <si>
+    <t>2.1 Advertisement partner information (name, email, phone number, address) may not be complete</t>
   </si>
 </sst>
 </file>
@@ -883,7 +996,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -923,12 +1036,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -998,12 +1105,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1039,9 +1140,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1363,16 +1461,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1432,7 +1530,7 @@
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20"/>
+      <c r="B12" s="18"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -1455,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D94B0A-294A-46CD-80A0-E82950B2698E}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,101 +1569,103 @@
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="58"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="60"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="33"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="49" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1575,50 +1675,46 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="12" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="15"/>
-    </row>
+      <c r="B13" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1631,7 +1727,7 @@
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A20" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{015B2D2F-AD0D-4D63-89DD-D5D3136F3C5C}"/>
+    <hyperlink ref="A18" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{015B2D2F-AD0D-4D63-89DD-D5D3136F3C5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1640,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79415FA7-6CDB-42D8-A113-D2105F582302}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,101 +1752,103 @@
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1760,55 +1858,46 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" ht="79.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="12" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B13" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1821,7 +1910,7 @@
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A21" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{C5DE00B5-2A2A-46DE-9D1B-639E52DF36C8}"/>
+    <hyperlink ref="A18" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{C5DE00B5-2A2A-46DE-9D1B-639E52DF36C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1832,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,101 +1935,103 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1951,25 +2042,27 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>100</v>
+      <c r="A12" s="23"/>
+      <c r="B12" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="41"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="39"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
+      <c r="B14" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="25"/>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1981,7 +2074,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2018,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA9D18-1CA4-4871-85B2-18BB43F4E55C}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C13"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,101 +2125,103 @@
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2137,26 +2232,30 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>102</v>
+      <c r="A12" s="23"/>
+      <c r="B12" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="41"/>
-    </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="39"/>
+    </row>
+    <row r="14" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="15"/>
+      <c r="B14" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="15" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2266,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2177,12 +2276,6 @@
     <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
@@ -2191,6 +2284,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
@@ -2204,8 +2303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FE8960-F0AE-4855-9BA4-1CED20B6740B}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,119 +2317,121 @@
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="36"/>
+      <c r="B6" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="48"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -2341,20 +2442,22 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="25"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2366,7 +2469,7 @@
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2403,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6806F9-C482-4A96-BD07-0DB8CFD37B42}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,101 +2520,103 @@
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2522,20 +2627,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>107</v>
+        <v>129</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="25"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2547,7 +2654,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2582,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED55F7-F44D-46F6-ADD5-ADA5945F102D}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,101 +2703,103 @@
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="49" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2701,20 +2810,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="25"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2726,7 +2837,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2761,8 +2872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D1CD4-D048-44CE-AE14-06222F52D34C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,101 +2886,103 @@
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2879,21 +2992,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+    <row r="12" spans="1:4" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="25"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2905,7 +3020,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2938,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B5A171-C8CF-457E-9DF8-6E96F6236BCA}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView topLeftCell="A11" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,101 +3069,103 @@
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3058,50 +3175,46 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="12" spans="1:4" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="15"/>
-    </row>
+      <c r="B13" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -3114,7 +3227,7 @@
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A20" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{4949DB17-DC8F-4FB9-BF87-4751256858C8}"/>
+    <hyperlink ref="A18" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{4949DB17-DC8F-4FB9-BF87-4751256858C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3123,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC3CBF5-E167-48E6-8768-D133250BF158}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,101 +3252,103 @@
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3243,55 +3358,46 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="12" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B13" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -3304,7 +3410,7 @@
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A21" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{325C37C0-617F-4D9B-A32D-771A43468D92}"/>
+    <hyperlink ref="A18" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{325C37C0-617F-4D9B-A32D-771A43468D92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Use Case Description and Activity Diagram
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666842CA-9DD2-4D7C-8926-0C3EF4D0D46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502EBB2-5B37-4713-8BF0-758FCF6F1C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="141">
   <si>
     <t>CONTENT</t>
   </si>
@@ -354,26 +354,8 @@
 3. Manager updates the status of the resignation request</t>
   </si>
   <si>
-    <t>1. Human resource department prompts to view employees
-2. Human resource departmen selects an employee to report
-3. Human resource department inputs the reason for the warning letter(reason)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Manager prompts to view warning letters
-2. Manager selects a warning letter proposal
-3. Manager updates the warning letter status </t>
-  </si>
-  <si>
-    <t>1.1 System displays a form asking for necessary employee information 
-2.1 System creates and saves a new employee</t>
-  </si>
-  <si>
     <t>1. Accounting and finance department prompts to view a list of employees whose salary change is accepted
 2. For each employee in the list, the accounting and finance updates their salary</t>
-  </si>
-  <si>
-    <t>1.1 System gets the list of employees whose salary change is accepted
-2.1 System updates and saves the salary change</t>
   </si>
   <si>
     <t>1. Movie front office prompts to view ongoing movies
@@ -383,15 +365,6 @@
 5. Movie front office selects the payment method and prompts to print ticket</t>
   </si>
   <si>
-    <t>1.1 System displays the form for creating a new 
-membership
-2.1 System creates and saves new employee</t>
-  </si>
-  <si>
-    <t>1.1 System displays the form to add a new supplier
-2.1 System creates and saves the new supplier</t>
-  </si>
-  <si>
     <t>1. Movie front office employee prompts to create a new membership
 2. Movie front office enters necessary customer information (name, gender, email, phone number, address, date of birth)</t>
   </si>
@@ -404,15 +377,6 @@
 2. External department employee fills the necessary informarion to add a new advertisement partner (name, email, phonenumber, address)</t>
   </si>
   <si>
-    <t>1.1 System displays the form to create a new advertisement partner
-2.1 System saves and creates the new advertisement partner</t>
-  </si>
-  <si>
-    <t>1.1 System gets all employees data
-2.1 System displays a form
-3.1 System will create and save a new warning letter proposal</t>
-  </si>
-  <si>
     <t>Human resource department proposes a warning letter by first retrieving a list of employees, then proceeds to select the employee to report along with the reason.</t>
   </si>
   <si>
@@ -441,9 +405,6 @@
   </si>
   <si>
     <t>External department employee creates and adds a new supplier by filling basic supplier  information</t>
-  </si>
-  <si>
-    <t>3.1. Reason is not filled by the human resource department</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -465,11 +426,6 @@
     <t>1.1 Warning letter proposals doesn't exist</t>
   </si>
   <si>
-    <t>1.1 Ongoing movies doesn't exist
-2.1 Schedule for a particular movie doesn’t exist
-3.1 Available seats for a movie schedule doesn't exist</t>
-  </si>
-  <si>
     <t>1.1 FnB items doesn't exist</t>
   </si>
   <si>
@@ -482,27 +438,48 @@
     <t>2.1 Advertisement partner information (name, email, phone number, address) may not be complete</t>
   </si>
   <si>
+    <t>1. Human resource department prompts to view employees
+2. Human resource department selects an employee to report
+3. Human resource department fills the warning letter proposal form (violationTime, violationDescription)</t>
+  </si>
+  <si>
+    <t>1.1 System gets all employees data
+2.1 System displays employaa data, along with a form
+3.1 System will create and save a new warning letter proposal
+3.2 System displays the submitted warning letter proposal form</t>
+  </si>
+  <si>
+    <t>3.1. Warning letter proposal form isn't fully filled</t>
+  </si>
+  <si>
     <t>1.1 System gets and displays the resignation requests
-2.1 System displays the resignation letter details
-3. 1 System updates and saves the status change</t>
+2.1 System displays the resignation request details
+3. 1 System updates and saves the status change
+3.2 System displays the updated resignation request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Manager prompts to view warning letters
+2. Manager selects a warning letter proposal
+3. Manager changes the warning letter status </t>
   </si>
   <si>
     <t>1.1 System gets and displays warning letter proposals
-2.1 System displays the details of the warning letter proposal, such as reason
-3.1 System updates and saves the warning letter status</t>
-  </si>
-  <si>
-    <t>1. Café front office employee prompts to view fnb 
-items
-2. Café front office employee selects the available items, according to customer's request
-3. Café front office selects a payment method and prompts to to create order</t>
-  </si>
-  <si>
-    <t>1.1 System gets and displays fnb items
-2.1 System calculates the total price
-2.2 System displays the total price
-2.3 System displays the available payment methods
-3.1 System saves and creates the order</t>
+2.1 System displays the details of the warning letter proposal, such as violationTime and vilationDescription
+3.1 System updates and saves the warning letter status
+3.2 System diplays changed warning letter proposal</t>
+  </si>
+  <si>
+    <t>1.1 System displays a form asking for necessary employee information 
+2.1 System creates and saves a new employee
+2.2 System displays newly created employee</t>
+  </si>
+  <si>
+    <t>1.1 System gets the list of employees whose salary change is accepted
+2.1 System updates and saves the salary change
+2.2 System displays the changed employee salary</t>
+  </si>
+  <si>
+    <t>1.1 Ongoing movies doesn't exist</t>
   </si>
   <si>
     <t>1.1 System gets and displays ongoing movies
@@ -510,11 +487,42 @@
 3.1 System displays the available seats for the selected movie schedule
 4.1 System calculates the total ticket price
 4.2 System displays the total ticket price and available payment methods
-5.1 System prints ticket
-5.2 System saves and records the ticket purchase</t>
-  </si>
-  <si>
-    <t>kkkjk</t>
+5.1 System saves and records the ticket purchase
+5.2 System prints ticket
+5.3 System displays printed ticket details</t>
+  </si>
+  <si>
+    <t>1. Café front office employee prompts to view fnb 
+items
+2. Café front office employee selects the available items, according to customer's request
+3. Café front office selects a payment method
+4. Café front office prompts to process order</t>
+  </si>
+  <si>
+    <t>1.1 System gets and displays fnb items
+2.1 System calculates the total price
+2.2 System displays the total price
+2.3 System displays the available payment methods
+3.1 System displays order details
+4.1 System saves and creates the order
+4.2 System prints receipt
+4.3 System displays newly created order</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form to add a new supplier
+2.1 System creates and saves the new supplier
+2.2 System displays newy created supplier</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form for creating a new 
+membership
+2.1 System creates and saves new employee
+2.2 System displays newly created membership</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form to create a new advertisement partner
+2.1 System saves and creates the new advertisement partner
+2.2 System displays newly created advertisement partner</t>
   </si>
 </sst>
 </file>
@@ -1557,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D94B0A-294A-46CD-80A0-E82950B2698E}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1619,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="15"/>
@@ -1680,10 +1688,10 @@
     <row r="12" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1691,16 +1699,12 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>141</v>
-      </c>
-    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1744,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79415FA7-6CDB-42D8-A113-D2105F582302}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,7 +1802,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -1867,10 +1871,10 @@
     <row r="12" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1878,7 +1882,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>
@@ -1927,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,7 +1985,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -2050,10 +2054,10 @@
     <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="36" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,7 +2070,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="15"/>
@@ -2117,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA9D18-1CA4-4871-85B2-18BB43F4E55C}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,7 +2175,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -2243,7 +2247,7 @@
         <v>100</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2256,11 +2260,11 @@
         <v>18</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2282,12 +2286,6 @@
     <row r="24" spans="1:1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
@@ -2296,6 +2294,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A19" location="Content!A1" display="BACK TO TABLE OF CONTENT" xr:uid="{F0A21BF0-B366-43B7-A8BF-0529B1B7FD33}"/>
@@ -2310,7 +2314,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,7 +2373,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="15"/>
@@ -2450,10 +2454,10 @@
     <row r="15" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="12" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2461,7 +2465,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="15"/>
@@ -2513,7 +2517,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,7 +2570,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -2635,10 +2639,10 @@
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2646,7 +2650,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>
@@ -2695,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED55F7-F44D-46F6-ADD5-ADA5945F102D}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,7 +2753,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -2818,10 +2822,10 @@
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2829,7 +2833,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>
@@ -2878,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D1CD4-D048-44CE-AE14-06222F52D34C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2932,7 +2936,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -2998,21 +3002,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>
@@ -3061,7 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B5A171-C8CF-457E-9DF8-6E96F6236BCA}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
@@ -3115,7 +3119,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -3181,13 +3185,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3195,7 +3199,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>
@@ -3244,8 +3248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC3CBF5-E167-48E6-8768-D133250BF158}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3298,7 +3302,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="15"/>
@@ -3367,10 +3371,10 @@
     <row r="12" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3378,7 +3382,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="15"/>

</xml_diff>

<commit_message>
Fixed Use Case Description and Activity Diagram
</commit_message>
<xml_diff>
--- a/Analysis/UseCaseDescription.xlsx
+++ b/Analysis/UseCaseDescription.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Stuck-in-the-Movie\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE00B947-ED50-43BF-95E4-4681BBF268C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50575492-6EFD-4B6E-89FD-62620F17A288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
-    <sheet name="01. Propose Warning Letter" sheetId="18" r:id="rId2"/>
-    <sheet name="02. Accept or Reject Resignatio" sheetId="2" r:id="rId3"/>
-    <sheet name="03. Approve or Disapprove Warni" sheetId="17" r:id="rId4"/>
+    <sheet name="01. Create Warning Letter" sheetId="18" r:id="rId2"/>
+    <sheet name="02. Update Resignation Letter S" sheetId="2" r:id="rId3"/>
+    <sheet name="03. Update Warning Letter Statu" sheetId="17" r:id="rId4"/>
     <sheet name="04. Add Employee" sheetId="19" r:id="rId5"/>
     <sheet name="05. Update Employee Salary" sheetId="20" r:id="rId6"/>
-    <sheet name="06. Create Ticket" sheetId="21" r:id="rId7"/>
+    <sheet name="06. Create Facility Equipment" sheetId="21" r:id="rId7"/>
     <sheet name="07. Create Food Beverage Order" sheetId="22" r:id="rId8"/>
     <sheet name="08. Create Membership" sheetId="24" r:id="rId9"/>
     <sheet name="09. Add Supplier" sheetId="25" r:id="rId10"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="146">
   <si>
     <t>CONTENT</t>
   </si>
@@ -124,27 +124,15 @@
     <t>BACK TO TABLE OF CONTENT</t>
   </si>
   <si>
-    <t>Propose Warning Letter</t>
-  </si>
-  <si>
     <t>Create Membership</t>
   </si>
   <si>
-    <t>Create Ticket</t>
-  </si>
-  <si>
     <t>Create Food/Beverage Order</t>
   </si>
   <si>
-    <t>Accept/Reject Resignation Request</t>
-  </si>
-  <si>
     <t>Manager accepts or rejects resignation request</t>
   </si>
   <si>
-    <t>Approve/Disapprove Warning Letter</t>
-  </si>
-  <si>
     <t>Human resource department proposes a warning letter</t>
   </si>
   <si>
@@ -157,12 +145,6 @@
     <t>Add Supplier</t>
   </si>
   <si>
-    <t>Add Advertisement Partner</t>
-  </si>
-  <si>
-    <t>Approve or Disapprove Warning Letter</t>
-  </si>
-  <si>
     <t>Manager approves or disapproves warning letter proposal</t>
   </si>
   <si>
@@ -172,36 +154,21 @@
     <t>Finance and accounting department changes employee salary</t>
   </si>
   <si>
-    <t>Movie front office division serves customer who wants to buy a ticket</t>
-  </si>
-  <si>
     <t>Café front office department serves customer who want to order snacks</t>
   </si>
   <si>
     <t>Movie front office division serves customer who wants to become a member</t>
   </si>
   <si>
-    <t>External department adds a new advertisement partner</t>
-  </si>
-  <si>
     <t>External division adds a new supplier</t>
   </si>
   <si>
     <t>Employee violated company rule</t>
   </si>
   <si>
-    <t>Manager sees/is notified by a resignation request</t>
-  </si>
-  <si>
-    <t>Manager sees/is notified by a warning letter approval request</t>
-  </si>
-  <si>
     <t>The human resource department accepted new employee/employees</t>
   </si>
   <si>
-    <t>Customer wants to buy a ticket, a movie front office employee serves them</t>
-  </si>
-  <si>
     <t>Customer wants to buy food/beverages, a café front office employee serves them</t>
   </si>
   <si>
@@ -214,9 +181,6 @@
     <t>Manager accepts salary change request by human resource department, the system forwards the data for further processing</t>
   </si>
   <si>
-    <t>External department wants to add a new advertisement partner</t>
-  </si>
-  <si>
     <t>Human resource department</t>
   </si>
   <si>
@@ -235,21 +199,6 @@
     <t>External department</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Submit Resignation Letter</t>
-  </si>
-  <si>
-    <t>Accept/Reject Salary Change, Propose Salary Change</t>
-  </si>
-  <si>
-    <t>View Shedule, Create Schedule, Update Schedule</t>
-  </si>
-  <si>
-    <t>View Food and Beverages</t>
-  </si>
-  <si>
     <t>Manager, Employee</t>
   </si>
   <si>
@@ -268,42 +217,16 @@
     <t>Accounting and finance</t>
   </si>
   <si>
-    <t>Accounting and finance, External</t>
-  </si>
-  <si>
     <t>Promotion and event, Manager</t>
   </si>
   <si>
     <t>Café kitchen division, Accounting and finance</t>
-  </si>
-  <si>
-    <t>Warning letter subsystem must be available</t>
   </si>
   <si>
     <t>Resignation request must exist.
 Resignation request subsystem must exist.</t>
   </si>
   <si>
-    <t>Warning letter must exist
-Warning letter subsytem must exist</t>
-  </si>
-  <si>
-    <t>Employee subsystem must exist</t>
-  </si>
-  <si>
-    <t>Employee must exist
-Employee subsystem must exist</t>
-  </si>
-  <si>
-    <t>Membership subsystem must exist</t>
-  </si>
-  <si>
-    <t>Supplier subsystem must exist</t>
-  </si>
-  <si>
-    <t>Advertisement partner subsystem must exist</t>
-  </si>
-  <si>
     <t>Warning letter must be created and saved</t>
   </si>
   <si>
@@ -314,24 +237,6 @@
   </si>
   <si>
     <t>Employee must be created and saved</t>
-  </si>
-  <si>
-    <t>Employee salary must be updates and saved</t>
-  </si>
-  <si>
-    <t>Ticket must be created, saved, and printed
-Available movie tickets must be updated
-Payment must be authenticated</t>
-  </si>
-  <si>
-    <t>Ticket subsystem must exist
-Movie schedule must be available
-Payment authorization services must be available</t>
-  </si>
-  <si>
-    <t>Food and beverages order subsystem must exist
-Food and beverge stock must be available
-Payment authorization services must be available</t>
   </si>
   <si>
     <t>Order must be created and saved
@@ -346,54 +251,19 @@
     <t>Supplier must be created and saved</t>
   </si>
   <si>
-    <t>Advertisement partner must be created and saved</t>
-  </si>
-  <si>
     <t>1. Manager prompts to view resignation requests
 2. Manager selects a resignation request
 3. Manager updates the status of the resignation request</t>
   </si>
   <si>
-    <t>1. Movie front office employee prompts to create a new membership
-2. Movie front office enters necessary customer information (name, gender, email, phone number, address, date of birth)</t>
-  </si>
-  <si>
     <t>1. External department employee prompts to add a new supplier
 2. External department employee fills the necessary information needed to add a new supplier (name, email, phone number, address)</t>
   </si>
   <si>
-    <t>1. External department employee prompts to add a new advertisement partner
-2. External department employee fills the necessary informarion to add a new advertisement partner (name, email, phonenumber, address)</t>
-  </si>
-  <si>
-    <t>Human resource department proposes a warning letter by first retrieving a list of employees, then proceeds to select the employee to report along with the reason.</t>
-  </si>
-  <si>
     <t>Manager retrieves a list of resignation requests, selects one of them and decides to accept or reject the request</t>
   </si>
   <si>
     <t>Manager receives a list of warning letter approval request, selects one of them, and decides to approve or disapprove the warning letter</t>
-  </si>
-  <si>
-    <t>Human resource department adds a new employee by entering basic employee information</t>
-  </si>
-  <si>
-    <t>Accounting and finance department gets a list of employees who salary change is accepted, and proceeds to update the salary based on the list</t>
-  </si>
-  <si>
-    <t>Movie front office division creates ticket by retrieving ongoing movies, selecting a movie, a schedule, seat number, and payment method.</t>
-  </si>
-  <si>
-    <t>Café front office employee creates a fnb order by selecting fnb items and payment type</t>
-  </si>
-  <si>
-    <t>Movie front office creates a new member by filling basic  information</t>
-  </si>
-  <si>
-    <t>External department employee creates and adds a new advertisement partner by filling basic advertisement partner information</t>
-  </si>
-  <si>
-    <t>External department employee creates and adds a new supplier by filling basic supplier  information</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -416,9 +286,6 @@
   </si>
   <si>
     <t>2.1 Supplier information (name, email, phone number, address) may be incomplete</t>
-  </si>
-  <si>
-    <t>2.1 Advertisement partner information (name, email, phone number, address) may not be complete</t>
   </si>
   <si>
     <t>1. Human resource department prompts to view employees
@@ -462,17 +329,6 @@
 2.2 System displays newy created supplier</t>
   </si>
   <si>
-    <t>1.1 System displays the form for creating a new 
-membership
-2.1 System creates and saves new employee
-2.2 System displays newly created membership</t>
-  </si>
-  <si>
-    <t>1.1 System displays the form to create a new advertisement partner
-2.1 System saves and creates the new advertisement partner
-2.2 System displays newly created advertisement partner</t>
-  </si>
-  <si>
     <t>1. Accounting and finance prompts to view employee salaries
 2. Accounting and finance selects an employee whose salary want to be changed
 3. Accounting and finance fills the salary change form (newSalary)</t>
@@ -487,33 +343,206 @@
     <t>3.1 The salary change form isn’t filled</t>
   </si>
   <si>
-    <t>1.1 System gets and displays ongoing movies
-2.1 System displays ticket purchase form
-3.1 System created ticket purchase
-3.2 System prints receipt
-3.3 System displays ticket purchase details</t>
-  </si>
-  <si>
-    <t>1. Movie front office prompts to view ongoing movies
-2. Movie front office selects movie
-3. Movie front office fills the ticket purchase form (movieSchedule, seats, paymentMethod, vouchers)</t>
-  </si>
-  <si>
-    <t>1.1 Ongoing movies doesn't exist
-3.1 Ticket purchase form isn't complete</t>
+    <t>Create Warning Letter</t>
+  </si>
+  <si>
+    <t>View Warning Letters Submitted, View Warning Letters Forwarded, Update Warning Letter Status, View 
+Personal Warning Letters</t>
+  </si>
+  <si>
+    <t>Update Resignation Letter Status</t>
+  </si>
+  <si>
+    <t>Create Resignation Letter, View Resignation Letters</t>
+  </si>
+  <si>
+    <t>Update Warning Letter Status</t>
+  </si>
+  <si>
+    <t>View Personal Warning Letters, View Warning Letters Forwarded, View Warning Letters Submitted,
+ Create Warning Letter</t>
+  </si>
+  <si>
+    <t>View Employee Report, View Employees, Update Employee, Update Employee Working Time, 
+View Employee Attendance, View Employee Personal Leave Requests, Update Employee Salary, View Employee Salaries</t>
+  </si>
+  <si>
+    <t>View Employee Salaries, Create Salary Change Proposal, View Salary Change List, View Salary 
+Change Proposal, Update Salary Change Proposal Status</t>
+  </si>
+  <si>
+    <t>View Membership, View Membership Report, Get Member Email</t>
+  </si>
+  <si>
+    <t>View Suppliers, Update Supplier</t>
+  </si>
+  <si>
+    <t>Employee subsystem must exist
+Employee information form's data must be complete</t>
+  </si>
+  <si>
+    <t>Warning letter subsystem must be available
+Warning letter proposal form's data must be complete</t>
+  </si>
+  <si>
+    <t>Supplier subsystem must exist
+Supplier information form's data must be complete</t>
+  </si>
+  <si>
+    <t>Manager sees a resignation request</t>
+  </si>
+  <si>
+    <t>Manager sees a warning letter approval request</t>
+  </si>
+  <si>
+    <t>Human resource department proposes a warning letter by first retrieving a list of employees, then proceeds to select the employee to report, and fills a warning letter form (violationTime, violationDescription).</t>
+  </si>
+  <si>
+    <t>Human resource department adds a new employee by entering employee information (name, gender, department, email, phonenumber, salary, address, date of birth)</t>
+  </si>
+  <si>
+    <t>Add Advertisement Partner</t>
+  </si>
+  <si>
+    <t>External department adds a new advertisement partner</t>
+  </si>
+  <si>
+    <t>External department wants to add a new advertisement partner</t>
+  </si>
+  <si>
+    <t>Advertisement partner must be created and saved</t>
+  </si>
+  <si>
+    <t>1. External department employee prompts to add a new advertisement partner
+2. External department employee fills the necessary informarion to add a new advertisement partner (name, email, phonenumber, address)</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form to create a new advertisement partner
+2.1 System saves and creates the new advertisement partner
+2.2 System displays newly created advertisement partner</t>
+  </si>
+  <si>
+    <t>2.1 Advertisement partner information (name, email, phone number, address) may not be complete</t>
+  </si>
+  <si>
+    <t>Advertisement partner subsystem must exist
+Add advertisement form's data must be complete</t>
+  </si>
+  <si>
+    <t>External department employee creates and adds a new advertisement partner by filling basic advertisement partner information (name, email, phonenumber, address)</t>
+  </si>
+  <si>
+    <t>Movie front office creates a new member by filling basic  information (name, gender, email, phone number, address, date of birth)</t>
+  </si>
+  <si>
+    <t>External department employee creates and adds a new supplier by filling basic supplier  information (name, email, phone number, address)</t>
+  </si>
+  <si>
+    <t>View Food and Beverages, Use Voucher, View Ongoing Order, Update Order Status, Create Membership</t>
+  </si>
+  <si>
+    <t>Food and beverages order subsystem must exist
+Food and beverge stock must be available
+Payment authorization services must be available
+Food and beverage purchase form's data must be complete</t>
+  </si>
+  <si>
+    <t>Employee must exist
+Employee subsystem must exist
+Salary change form's data must be complete</t>
+  </si>
+  <si>
+    <t>Warning letter subsystem must be available
+Warning letter must exist</t>
+  </si>
+  <si>
+    <t>Accounting and finance department gets a list of employees who salary change is accepted, and proceeds to update the salary based on the list by selecting a particular employee whose salary want to be changed, and filling employee salary change form (newSalary)</t>
+  </si>
+  <si>
+    <t>View Advertisement Partner, Update Advertsement Partner</t>
+  </si>
+  <si>
+    <t>Employee salary must be updated and saved</t>
+  </si>
+  <si>
+    <t>Create Facility/Equipment</t>
+  </si>
+  <si>
+    <t>Storage department records newly purchased item into the system</t>
+  </si>
+  <si>
+    <t>Employee facility/equipment request is approved</t>
+  </si>
+  <si>
+    <t>Storage Department</t>
+  </si>
+  <si>
+    <t>View Facility and Equipment</t>
+  </si>
+  <si>
+    <t>Accounting and Finance Department, Concerned Employee</t>
+  </si>
+  <si>
+    <t>System saves the newly created facility/equipment</t>
+  </si>
+  <si>
+    <t>1. Storage department prompts to add new item
+2. Storage department fill the necessary item information (itemName, itemDescription)</t>
+  </si>
+  <si>
+    <t>1.1 System displays facility/equipment creation form
+2.1 System saves the newly added item
+2.2 System prints item label
+2.3 System displays item details</t>
+  </si>
+  <si>
+    <t>Storage department records the newly purchased facility/equipment into the system by filling necessary information (itemName, itemDescription)</t>
+  </si>
+  <si>
+    <t>Concerned employee's item is available
+Facility/Equipmet subsystem must exist
+Facility/Equipment form's data must exist</t>
+  </si>
+  <si>
+    <t>2.1 Newly added item's information (itemName, itemDescription) is incomplete</t>
+  </si>
+  <si>
+    <t>Accounting and finance, External, Café Kitchen Division</t>
   </si>
   <si>
     <t>1. Cafe front office prompts to view order form
-2. Cafe front office fills the food and beverage purchase form (FoodAndBeverageItems, paymentMethod, voucher)</t>
-  </si>
-  <si>
-    <t>2.1 Food and beverage purchase form isn't complete</t>
-  </si>
-  <si>
-    <t>1.1 System displays food and beverage purchase form
-2.1 System creates food and beverage order
-2.2 System prints receipt
-2.3 System displays food and beverage order details</t>
+2. Cafe front office fills the food and beverage purchase form (FoodAndBeverageItems, paymentMethod, voucher)
+3. Café front office scans membership card if needed, and prompts to finalize order</t>
+  </si>
+  <si>
+    <t>1.1 System gets available foods and beverages
+1.2 System displays food and beverage order form
+2.1 System prompts to input member card
+3.1 System calculates customer's order
+3.2 System adds member points if needed
+3.3 System creates and saves FnB order
+3.4 System prints receipt
+3.5 System displays order details</t>
+  </si>
+  <si>
+    <t>Café front office employee creates a fnb order by selecting fnb items, payment method, voucher if available, and membership card if available</t>
+  </si>
+  <si>
+    <t>1. Movie front office employee prompts to create a new membership
+2. Movie front office enters necessary customer information (name, gender, email, phone number, address, date of birth)
+3. Movie front office selects a payment method and prompts to finalize membership creation</t>
+  </si>
+  <si>
+    <t>1.1 System displays the form for creating a new 
+membership
+2.1 System prompts payment method
+3.1 System creates and saves new membership
+3.2 System prints membership card
+3.3 System displays membership details</t>
+  </si>
+  <si>
+    <t>1.1 Food and beverages doesn't exist
+2.1 Food and beverage purchase form isn’t complete</t>
   </si>
 </sst>
 </file>
@@ -609,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -992,12 +1021,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1043,6 +1081,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1107,13 +1151,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1133,12 +1177,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1153,6 +1191,24 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1462,16 +1518,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1556,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D94B0A-294A-46CD-80A0-E82950B2698E}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,7 +1627,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="53"/>
     </row>
@@ -1580,7 +1636,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="14"/>
@@ -1589,84 +1645,84 @@
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="33"/>
+      <c r="B3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="35"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="33"/>
+      <c r="B5" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="35"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="33"/>
+      <c r="B10" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="35"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1677,22 +1733,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="12" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1739,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79415FA7-6CDB-42D8-A113-D2105F582302}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,19 +1809,19 @@
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1773,83 +1829,83 @@
         <v>13</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="29"/>
+        <v>110</v>
+      </c>
+      <c r="C3" s="31"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1860,22 +1916,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1922,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028246F-37F7-4539-895E-D5AB51AE2662}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,103 +1992,103 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2043,27 +2099,27 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>123</v>
+      <c r="A12" s="25"/>
+      <c r="B12" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="39"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="41"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="25"/>
+      <c r="B14" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="27"/>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2112,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA9D18-1CA4-4871-85B2-18BB43F4E55C}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,103 +2182,103 @@
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2233,29 +2289,29 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="39"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="41"/>
     </row>
     <row r="14" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="25"/>
+      <c r="B14" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2304,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FE8960-F0AE-4855-9BA4-1CED20B6740B}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,121 +2374,121 @@
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="44"/>
+      <c r="B4" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="46"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
+    <row r="5" spans="1:4" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="44"/>
+      <c r="B11" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="46"/>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -2442,23 +2498,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+    <row r="15" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
       <c r="B15" s="12" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="25"/>
+      <c r="B16" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="27"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2507,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6806F9-C482-4A96-BD07-0DB8CFD37B42}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,103 +2577,103 @@
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2628,22 +2684,22 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2688,10 +2744,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED55F7-F44D-46F6-ADD5-ADA5945F102D}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,107 +2756,110 @@
     <col min="2" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="31"/>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="33"/>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="36"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="34"/>
+      <c r="B6" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="B7" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="36"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2810,28 +2869,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+    <row r="12" spans="1:7" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
       <c r="B12" s="12" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>27</v>
@@ -2871,10 +2930,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D1CD4-D048-44CE-AE14-06222F52D34C}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,107 +2942,139 @@
     <col min="2" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2993,28 +3084,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
       <c r="B12" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>27</v>
@@ -3054,10 +3145,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B5A171-C8CF-457E-9DF8-6E96F6236BCA}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3066,107 +3157,140 @@
     <col min="2" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+    </row>
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+    </row>
+    <row r="9" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+    </row>
+    <row r="10" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="E10" s="61"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3176,28 +3300,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:8" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
       <c r="B12" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>27</v>
@@ -3237,10 +3361,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC3CBF5-E167-48E6-8768-D133250BF158}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3249,107 +3373,119 @@
     <col min="2" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="36"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="36"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="34"/>
+      <c r="B10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3359,28 +3495,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:6" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
       <c r="B12" s="12" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" s="25"/>
+      <c r="B13" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>27</v>

</xml_diff>